<commit_message>
Update README with sample description and refresh Budget_Tracker_2025.xlsx
</commit_message>
<xml_diff>
--- a/assets/Budget_Tracker_2025.xlsx
+++ b/assets/Budget_Tracker_2025.xlsx
@@ -503,7 +503,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <font/>
       <fill>
@@ -540,6 +540,22 @@
         </patternFill>
       </fill>
       <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFC7CE"/>
+          <bgColor rgb="00FFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00C6EFCE"/>
+          <bgColor rgb="00C6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
@@ -747,7 +763,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -821,7 +837,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -844,7 +860,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
         </a:p>
       </txPr>
@@ -1367,7 +1383,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
         </a:p>
       </txPr>
@@ -1505,7 +1521,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1579,7 +1595,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1602,7 +1618,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
         </a:p>
       </txPr>
@@ -1941,37 +1957,37 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="35" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="35" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="35" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="35" t="inlineStr">
         <is>
           <t>Days Until Due</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="35" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="35" t="inlineStr">
         <is>
           <t>Paid?</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="35" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
@@ -2016,28 +2032,28 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="38" t="n">
         <v>96.19</v>
       </c>
-      <c r="D2" s="9" t="inlineStr">
+      <c r="D2" s="38" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="G2" s="9" t="inlineStr">
+      <c r="G2" s="38" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H2" s="9" t="n"/>
+      <c r="H2" s="38" t="n"/>
       <c r="I2" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2077,28 +2093,28 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="38" t="n">
         <v>181.75</v>
       </c>
-      <c r="D3" s="15" t="inlineStr">
+      <c r="D3" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="15" t="inlineStr">
+      <c r="F3" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="G3" s="15" t="inlineStr">
+      <c r="G3" s="41" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H3" s="9" t="n"/>
+      <c r="H3" s="38" t="n"/>
       <c r="I3" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2132,12 +2148,12 @@
     <row r="4" hidden="1" s="57">
       <c r="A4" s="26" t="n"/>
       <c r="B4" s="18" t="n"/>
-      <c r="C4" s="9" t="n"/>
-      <c r="D4" s="9" t="n"/>
-      <c r="E4" s="9" t="n"/>
-      <c r="F4" s="9" t="n"/>
-      <c r="G4" s="9" t="n"/>
-      <c r="H4" s="9" t="n"/>
+      <c r="C4" s="38" t="n"/>
+      <c r="D4" s="38" t="n"/>
+      <c r="E4" s="38" t="n"/>
+      <c r="F4" s="38" t="n"/>
+      <c r="G4" s="38" t="n"/>
+      <c r="H4" s="38" t="n"/>
       <c r="I4" s="19">
         <f>IF(AND(A4&gt;=TODAY(), A4&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2175,28 +2191,28 @@
           <t>Car Payment</t>
         </is>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="38" t="n">
         <v>547.9</v>
       </c>
-      <c r="D5" s="9" t="inlineStr">
+      <c r="D5" s="38" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="9" t="inlineStr">
+      <c r="F5" s="38" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G5" s="9" t="inlineStr">
+      <c r="G5" s="38" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H5" s="9" t="n"/>
+      <c r="H5" s="38" t="n"/>
       <c r="I5" s="19">
         <f>IF(AND(A5&gt;=TODAY(), A5&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2234,28 +2250,28 @@
           <t>Rent Plan (Back)</t>
         </is>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="38" t="n">
         <v>142</v>
       </c>
-      <c r="D6" s="15" t="inlineStr">
+      <c r="D6" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="15" t="inlineStr">
+      <c r="F6" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="G6" s="15" t="inlineStr">
+      <c r="G6" s="41" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H6" s="9" t="n"/>
+      <c r="H6" s="38" t="n"/>
       <c r="I6" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -2295,24 +2311,24 @@
           <t>affirm</t>
         </is>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="38" t="n">
         <v>36.46</v>
       </c>
-      <c r="D7" s="15" t="inlineStr">
+      <c r="D7" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E7" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="15" t="n"/>
-      <c r="G7" s="15" t="inlineStr">
+      <c r="F7" s="41" t="n"/>
+      <c r="G7" s="41" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H7" s="9" t="n"/>
+      <c r="H7" s="38" t="n"/>
       <c r="I7" s="23">
         <f>IF(AND(A7&gt;=TODAY(), A7&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2350,24 +2366,24 @@
           <t>affirm</t>
         </is>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="38" t="n">
         <v>86.09</v>
       </c>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="D8" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E8" s="9" t="n">
+      <c r="E8" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="9" t="n"/>
-      <c r="G8" s="9" t="inlineStr">
+      <c r="F8" s="38" t="n"/>
+      <c r="G8" s="38" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H8" s="9" t="n"/>
+      <c r="H8" s="38" t="n"/>
       <c r="I8" s="19">
         <f>IF(AND(A8&gt;=TODAY(), A8&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2405,24 +2421,24 @@
           <t xml:space="preserve">Rent  </t>
         </is>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="38" t="n">
         <v>2004</v>
       </c>
-      <c r="D9" s="15" t="inlineStr">
+      <c r="D9" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E9" s="9" t="n">
+      <c r="E9" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="15" t="n"/>
-      <c r="G9" s="15" t="inlineStr">
+      <c r="F9" s="41" t="n"/>
+      <c r="G9" s="41" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H9" s="9" t="n"/>
+      <c r="H9" s="38" t="n"/>
       <c r="I9" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2455,16 +2471,16 @@
     <row r="10" hidden="1" s="57">
       <c r="A10" s="26" t="n"/>
       <c r="B10" s="18" t="n"/>
-      <c r="C10" s="9" t="n"/>
-      <c r="D10" s="15" t="inlineStr">
+      <c r="C10" s="38" t="n"/>
+      <c r="D10" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-      <c r="G10" s="9" t="n"/>
-      <c r="H10" s="9" t="n"/>
+      <c r="E10" s="38" t="n"/>
+      <c r="F10" s="38" t="n"/>
+      <c r="G10" s="38" t="n"/>
+      <c r="H10" s="38" t="n"/>
       <c r="I10" s="19">
         <f>IF(AND(A10&gt;=TODAY(), A10&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2502,28 +2518,28 @@
           <t>Flight Ticket</t>
         </is>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="38" t="n">
         <v>1200</v>
       </c>
-      <c r="D11" s="15" t="inlineStr">
+      <c r="D11" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="38" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G11" s="9" t="inlineStr">
+      <c r="G11" s="38" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="H11" s="9" t="n"/>
+      <c r="H11" s="38" t="n"/>
       <c r="I11" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2562,28 +2578,28 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="38" t="n">
         <v>86.09</v>
       </c>
-      <c r="D12" s="15" t="inlineStr">
+      <c r="D12" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E12" s="9" t="n">
+      <c r="E12" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="F12" s="15" t="inlineStr">
+      <c r="F12" s="41" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G12" s="15" t="inlineStr">
+      <c r="G12" s="41" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="H12" s="9" t="n"/>
+      <c r="H12" s="38" t="n"/>
       <c r="I12" s="23">
         <f>IF(AND(A12&gt;=TODAY(), A12&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2621,28 +2637,28 @@
           <t>October Rent</t>
         </is>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="38" t="n">
         <v>2052.09</v>
       </c>
-      <c r="D13" s="15" t="inlineStr">
+      <c r="D13" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E13" s="9" t="n">
+      <c r="E13" s="38" t="n">
         <v>9</v>
       </c>
-      <c r="F13" s="9" t="inlineStr">
+      <c r="F13" s="38" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G13" s="9" t="inlineStr">
+      <c r="G13" s="38" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H13" s="9" t="n"/>
+      <c r="H13" s="38" t="n"/>
       <c r="I13" s="19">
         <f>IF(AND(A13&gt;=TODAY(), A13&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2680,28 +2696,28 @@
           <t>Capital One</t>
         </is>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="38" t="n">
         <v>200</v>
       </c>
-      <c r="D14" s="15" t="inlineStr">
+      <c r="D14" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E14" s="9" t="n">
+      <c r="E14" s="38" t="n">
         <v>18</v>
       </c>
-      <c r="F14" s="15" t="inlineStr">
+      <c r="F14" s="41" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G14" s="15" t="inlineStr">
+      <c r="G14" s="41" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H14" s="9" t="n"/>
+      <c r="H14" s="38" t="n"/>
       <c r="I14" s="23">
         <f>IF(AND(A14&gt;=TODAY(), A14&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2739,15 +2755,15 @@
           <t>FPL</t>
         </is>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="38" t="n">
         <v>50.12</v>
       </c>
-      <c r="D15" s="15" t="inlineStr">
+      <c r="D15" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E15" s="9" t="n">
+      <c r="E15" s="38" t="n">
         <v>16</v>
       </c>
       <c r="F15" s="19" t="inlineStr">
@@ -2760,7 +2776,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H15" s="9" t="n"/>
+      <c r="H15" s="38" t="n"/>
       <c r="I15" s="19">
         <f>IF(AND(A15&gt;=TODAY(), A15&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2798,15 +2814,15 @@
           <t>Mazda</t>
         </is>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="38" t="n">
         <v>308</v>
       </c>
-      <c r="D16" s="15" t="inlineStr">
+      <c r="D16" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E16" s="9" t="n">
+      <c r="E16" s="38" t="n">
         <v>28</v>
       </c>
       <c r="F16" s="23" t="inlineStr">
@@ -2819,7 +2835,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H16" s="9" t="n"/>
+      <c r="H16" s="38" t="n"/>
       <c r="I16" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2858,15 +2874,15 @@
           <t>Mariner</t>
         </is>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="38" t="n">
         <v>359</v>
       </c>
-      <c r="D17" s="9" t="inlineStr">
+      <c r="D17" s="38" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E17" s="9" t="n">
+      <c r="E17" s="38" t="n">
         <v>28</v>
       </c>
       <c r="F17" s="19" t="inlineStr">
@@ -2879,7 +2895,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H17" s="9" t="n"/>
+      <c r="H17" s="38" t="n"/>
       <c r="I17" s="19">
         <f>IF(AND(A17&gt;=TODAY(), A17&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2917,15 +2933,15 @@
           <t>JVT</t>
         </is>
       </c>
-      <c r="C18" s="9" t="n">
+      <c r="C18" s="38" t="n">
         <v>312</v>
       </c>
-      <c r="D18" s="15" t="inlineStr">
+      <c r="D18" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E18" s="9" t="n">
+      <c r="E18" s="38" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="23" t="inlineStr">
@@ -2938,7 +2954,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H18" s="9" t="n"/>
+      <c r="H18" s="38" t="n"/>
       <c r="I18" s="23">
         <f>IF(AND(A18&gt;=TODAY(), A18&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2976,15 +2992,15 @@
           <t>Miscellaneous</t>
         </is>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="38" t="n">
         <v>89</v>
       </c>
-      <c r="D19" s="9" t="inlineStr">
+      <c r="D19" s="38" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E19" s="9" t="n">
+      <c r="E19" s="38" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="19" t="inlineStr">
@@ -2997,7 +3013,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H19" s="9" t="n"/>
+      <c r="H19" s="38" t="n"/>
       <c r="I19" s="19">
         <f>IF(AND(A19&gt;=TODAY(), A19&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3035,15 +3051,15 @@
           <t>Progressive</t>
         </is>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="38" t="n">
         <v>179.66</v>
       </c>
-      <c r="D20" s="15" t="inlineStr">
+      <c r="D20" s="41" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E20" s="9" t="n">
+      <c r="E20" s="38" t="n">
         <v>4</v>
       </c>
       <c r="F20" s="23" t="inlineStr">
@@ -3056,7 +3072,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H20" s="9" t="n"/>
+      <c r="H20" s="38" t="n"/>
       <c r="I20" s="23">
         <f>IF(AND(A20&gt;=TODAY(), A20&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3094,15 +3110,15 @@
           <t>Alliance</t>
         </is>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="38" t="n">
         <v>151</v>
       </c>
-      <c r="D21" s="9" t="inlineStr">
+      <c r="D21" s="38" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E21" s="9" t="n">
+      <c r="E21" s="38" t="n">
         <v>4</v>
       </c>
       <c r="F21" s="19" t="inlineStr">
@@ -3115,7 +3131,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H21" s="9" t="n"/>
+      <c r="H21" s="38" t="n"/>
       <c r="I21" s="19">
         <f>IF(AND(A21&gt;=TODAY(), A21&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3153,15 +3169,15 @@
           <t>Sloan</t>
         </is>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="38" t="n">
         <v>150.75</v>
       </c>
-      <c r="D22" s="15" t="inlineStr">
+      <c r="D22" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E22" s="9" t="n">
+      <c r="E22" s="38" t="n">
         <v>35</v>
       </c>
       <c r="F22" s="23" t="inlineStr">
@@ -3174,7 +3190,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H22" s="9" t="n"/>
+      <c r="H22" s="38" t="n"/>
       <c r="I22" s="23">
         <f>IF(AND(A22&gt;=TODAY(), A22&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3212,15 +3228,15 @@
           <t>Fortina</t>
         </is>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="38" t="n">
         <v>40</v>
       </c>
-      <c r="D23" s="9" t="inlineStr">
+      <c r="D23" s="38" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E23" s="9" t="n">
+      <c r="E23" s="38" t="n">
         <v>0</v>
       </c>
       <c r="F23" s="19" t="inlineStr">
@@ -3233,7 +3249,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H23" s="9" t="n"/>
+      <c r="H23" s="38" t="n"/>
       <c r="I23" s="19">
         <f>IF(AND(A23&gt;=TODAY(), A23&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3271,15 +3287,15 @@
           <t>Mariner</t>
         </is>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="38" t="n">
         <v>359</v>
       </c>
-      <c r="D24" s="15" t="inlineStr">
+      <c r="D24" s="41" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E24" s="9" t="n">
+      <c r="E24" s="38" t="n">
         <v>30</v>
       </c>
       <c r="F24" s="23" t="inlineStr">
@@ -3292,7 +3308,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H24" s="9" t="n"/>
+      <c r="H24" s="38" t="n"/>
       <c r="I24" s="23">
         <f>IF(AND(A24&gt;=TODAY(), A24&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3330,15 +3346,15 @@
           <t>Adjustment</t>
         </is>
       </c>
-      <c r="C25" s="9" t="n">
+      <c r="C25" s="38" t="n">
         <v>652</v>
       </c>
-      <c r="D25" s="9" t="inlineStr">
+      <c r="D25" s="38" t="inlineStr">
         <is>
           <t>low</t>
         </is>
       </c>
-      <c r="E25" s="9" t="n">
+      <c r="E25" s="38" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="19" t="n"/>
@@ -3347,7 +3363,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H25" s="9" t="n"/>
+      <c r="H25" s="38" t="n"/>
       <c r="I25" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -3386,15 +3402,15 @@
           <t>Progressive</t>
         </is>
       </c>
-      <c r="C26" s="9" t="n">
+      <c r="C26" s="38" t="n">
         <v>179</v>
       </c>
-      <c r="D26" s="15" t="inlineStr">
+      <c r="D26" s="41" t="inlineStr">
         <is>
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E26" s="9" t="n">
+      <c r="E26" s="38" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="23" t="n"/>
@@ -3403,7 +3419,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H26" s="9" t="n"/>
+      <c r="H26" s="38" t="n"/>
       <c r="I26" s="23">
         <f>IF(AND(A26&gt;=TODAY(), A26&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3441,16 +3457,16 @@
           <t>Alliance</t>
         </is>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="38">
         <f>155+25</f>
         <v/>
       </c>
-      <c r="D27" s="9" t="inlineStr">
+      <c r="D27" s="38" t="inlineStr">
         <is>
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E27" s="9" t="n">
+      <c r="E27" s="38" t="n">
         <v>1</v>
       </c>
       <c r="F27" s="19" t="n"/>
@@ -3459,7 +3475,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H27" s="9" t="n"/>
+      <c r="H27" s="38" t="n"/>
       <c r="I27" s="19">
         <f>IF(AND(A27&gt;=TODAY(), A27&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3497,15 +3513,15 @@
           <t>car</t>
         </is>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="38" t="n">
         <v>547.9</v>
       </c>
-      <c r="D28" s="15" t="inlineStr">
+      <c r="D28" s="41" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E28" s="9" t="n">
+      <c r="E28" s="38" t="n">
         <v>12</v>
       </c>
       <c r="F28" s="23" t="inlineStr">
@@ -3518,7 +3534,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H28" s="9" t="n"/>
+      <c r="H28" s="38" t="n"/>
       <c r="I28" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -3557,15 +3573,15 @@
           <t>Rent</t>
         </is>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="38" t="n">
         <v>603</v>
       </c>
-      <c r="D29" s="9" t="inlineStr">
+      <c r="D29" s="38" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E29" s="9" t="n">
+      <c r="E29" s="38" t="n">
         <v>16</v>
       </c>
       <c r="F29" s="19" t="inlineStr">
@@ -3578,7 +3594,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H29" s="9" t="n"/>
+      <c r="H29" s="38" t="n"/>
       <c r="I29" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -3617,15 +3633,15 @@
           <t>Newera</t>
         </is>
       </c>
-      <c r="C30" s="9" t="n">
+      <c r="C30" s="38" t="n">
         <v>303</v>
       </c>
-      <c r="D30" s="15" t="inlineStr">
+      <c r="D30" s="41" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E30" s="9" t="n">
+      <c r="E30" s="38" t="n">
         <v>5</v>
       </c>
       <c r="F30" s="23" t="inlineStr">
@@ -3638,7 +3654,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H30" s="9" t="n"/>
+      <c r="H30" s="38" t="n"/>
       <c r="I30" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -3677,15 +3693,15 @@
           <t>Capital One</t>
         </is>
       </c>
-      <c r="C31" s="9" t="n">
+      <c r="C31" s="38" t="n">
         <v>200</v>
       </c>
-      <c r="D31" s="15" t="inlineStr">
+      <c r="D31" s="41" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E31" s="9" t="n">
+      <c r="E31" s="38" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="19" t="inlineStr">
@@ -3698,7 +3714,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H31" s="9" t="n"/>
+      <c r="H31" s="38" t="n"/>
       <c r="I31" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -3737,7 +3753,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C32" s="9" t="n">
+      <c r="C32" s="38" t="n">
         <v>181.75</v>
       </c>
       <c r="D32" s="23" t="inlineStr">
@@ -3745,7 +3761,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E32" s="9" t="n">
+      <c r="E32" s="38" t="n">
         <v>14</v>
       </c>
       <c r="F32" s="19" t="inlineStr">
@@ -3758,7 +3774,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H32" s="9" t="n"/>
+      <c r="H32" s="38" t="n"/>
       <c r="I32" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve"> no</t>
@@ -3797,7 +3813,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C33" s="9" t="n">
+      <c r="C33" s="38" t="n">
         <v>36.46</v>
       </c>
       <c r="D33" s="19" t="inlineStr">
@@ -3805,7 +3821,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E33" s="9" t="n">
+      <c r="E33" s="38" t="n">
         <v>14</v>
       </c>
       <c r="F33" s="19" t="inlineStr">
@@ -3818,7 +3834,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H33" s="9" t="n"/>
+      <c r="H33" s="38" t="n"/>
       <c r="I33" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -3857,7 +3873,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C34" s="9" t="n">
+      <c r="C34" s="38" t="n">
         <v>86.09</v>
       </c>
       <c r="D34" s="23" t="inlineStr">
@@ -3865,7 +3881,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E34" s="9" t="n">
+      <c r="E34" s="38" t="n">
         <v>14</v>
       </c>
       <c r="F34" s="19" t="inlineStr">
@@ -3878,7 +3894,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H34" s="9" t="n"/>
+      <c r="H34" s="38" t="n"/>
       <c r="I34" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -3917,7 +3933,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C35" s="9" t="n">
+      <c r="C35" s="38" t="n">
         <v>96.19</v>
       </c>
       <c r="D35" s="19" t="inlineStr">
@@ -3925,7 +3941,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E35" s="9" t="n">
+      <c r="E35" s="38" t="n">
         <v>14</v>
       </c>
       <c r="F35" s="19" t="inlineStr">
@@ -3938,7 +3954,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H35" s="9" t="n"/>
+      <c r="H35" s="38" t="n"/>
       <c r="I35" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -3977,7 +3993,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C36" s="9" t="n">
+      <c r="C36" s="38" t="n">
         <v>55.57</v>
       </c>
       <c r="D36" s="23" t="inlineStr">
@@ -3985,7 +4001,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E36" s="9" t="n">
+      <c r="E36" s="38" t="n">
         <v>14</v>
       </c>
       <c r="F36" s="19" t="inlineStr">
@@ -3998,7 +4014,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H36" s="9" t="n"/>
+      <c r="H36" s="38" t="n"/>
       <c r="I36" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -4037,7 +4053,7 @@
           <t>Rent</t>
         </is>
       </c>
-      <c r="C37" s="9" t="n">
+      <c r="C37" s="38" t="n">
         <v>142</v>
       </c>
       <c r="D37" s="19" t="inlineStr">
@@ -4045,7 +4061,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E37" s="9" t="n">
+      <c r="E37" s="38" t="n">
         <v>16</v>
       </c>
       <c r="F37" s="19" t="inlineStr">
@@ -4058,7 +4074,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H37" s="9" t="n"/>
+      <c r="H37" s="38" t="n"/>
       <c r="I37" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -4097,7 +4113,7 @@
           <t>Mariner</t>
         </is>
       </c>
-      <c r="C38" s="9" t="n">
+      <c r="C38" s="38" t="n">
         <v>359</v>
       </c>
       <c r="D38" s="23" t="inlineStr">
@@ -4105,7 +4121,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E38" s="9" t="n">
+      <c r="E38" s="38" t="n">
         <v>16</v>
       </c>
       <c r="F38" s="23" t="n"/>
@@ -4114,7 +4130,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H38" s="9" t="n"/>
+      <c r="H38" s="38" t="n"/>
       <c r="I38" s="23">
         <f>IF(AND(A38&gt;=TODAY(), A38&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -4152,7 +4168,7 @@
           <t>Power</t>
         </is>
       </c>
-      <c r="C39" s="9" t="n">
+      <c r="C39" s="38" t="n">
         <v>0</v>
       </c>
       <c r="D39" s="19" t="inlineStr">
@@ -4160,7 +4176,7 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="E39" s="9" t="n">
+      <c r="E39" s="38" t="n">
         <v>0</v>
       </c>
       <c r="F39" s="19" t="inlineStr">
@@ -4173,7 +4189,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H39" s="9" t="n"/>
+      <c r="H39" s="38" t="n"/>
       <c r="I39" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -4212,7 +4228,7 @@
           <t>Cable</t>
         </is>
       </c>
-      <c r="C40" s="9" t="n">
+      <c r="C40" s="38" t="n">
         <v>0</v>
       </c>
       <c r="D40" s="23" t="inlineStr">
@@ -4220,7 +4236,7 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="E40" s="9" t="n">
+      <c r="E40" s="38" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="23" t="inlineStr">
@@ -4233,7 +4249,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H40" s="9" t="n"/>
+      <c r="H40" s="38" t="n"/>
       <c r="I40" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -4273,7 +4289,7 @@
           <t>Ticket</t>
         </is>
       </c>
-      <c r="C41" s="9" t="n">
+      <c r="C41" s="38" t="n">
         <v>1200</v>
       </c>
       <c r="D41" s="19" t="inlineStr">
@@ -4281,7 +4297,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E41" s="9" t="n">
+      <c r="E41" s="38" t="n">
         <v>14</v>
       </c>
       <c r="F41" s="19" t="inlineStr">
@@ -4294,7 +4310,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H41" s="9" t="n"/>
+      <c r="H41" s="38" t="n"/>
       <c r="I41" s="19" t="inlineStr">
         <is>
           <t>np</t>
@@ -4328,12 +4344,12 @@
     <row r="42" ht="15.75" customHeight="1" s="57">
       <c r="A42" s="26" t="n"/>
       <c r="B42" s="27" t="n"/>
-      <c r="C42" s="9" t="n"/>
+      <c r="C42" s="38" t="n"/>
       <c r="D42" s="23" t="n"/>
-      <c r="E42" s="9" t="n"/>
+      <c r="E42" s="38" t="n"/>
       <c r="F42" s="23" t="n"/>
       <c r="G42" s="23" t="n"/>
-      <c r="H42" s="9" t="n"/>
+      <c r="H42" s="38" t="n"/>
       <c r="I42" s="23">
         <f>IF(AND(A42&gt;=TODAY(), A42&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -4364,14 +4380,14 @@
     </row>
     <row r="43" ht="15.75" customHeight="1" s="57">
       <c r="A43" s="26" t="n"/>
-      <c r="B43" s="9" t="n"/>
-      <c r="C43" s="9" t="n"/>
+      <c r="B43" s="38" t="n"/>
+      <c r="C43" s="38" t="n"/>
       <c r="D43" s="19" t="n"/>
-      <c r="E43" s="9" t="n"/>
+      <c r="E43" s="38" t="n"/>
       <c r="F43" s="19" t="n"/>
       <c r="G43" s="23" t="n"/>
-      <c r="H43" s="9" t="n"/>
-      <c r="I43" s="9">
+      <c r="H43" s="38" t="n"/>
+      <c r="I43" s="38">
         <f>IF(AND(A43&gt;=TODAY(), A43&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
       </c>
@@ -4402,12 +4418,12 @@
     <row r="44" ht="15.75" customHeight="1" s="57">
       <c r="A44" s="26" t="n"/>
       <c r="B44" s="21" t="n"/>
-      <c r="C44" s="9" t="n"/>
-      <c r="D44" s="9" t="n"/>
-      <c r="E44" s="9" t="n"/>
-      <c r="F44" s="9" t="n"/>
+      <c r="C44" s="38" t="n"/>
+      <c r="D44" s="38" t="n"/>
+      <c r="E44" s="38" t="n"/>
+      <c r="F44" s="38" t="n"/>
       <c r="G44" s="23" t="n"/>
-      <c r="H44" s="9" t="n"/>
+      <c r="H44" s="38" t="n"/>
       <c r="I44" s="21" t="n"/>
       <c r="J44" s="20" t="n"/>
       <c r="K44" s="17">
@@ -31675,7 +31691,10 @@
         <f>SUM(Income!C2:C100)</f>
         <v/>
       </c>
-      <c r="C2" s="5" t="n"/>
+      <c r="C2" s="5">
+        <f>SPARKLINE('Monthly Summary'!B2:B100, {"charttype","line"; "color","blue"})</f>
+        <v/>
+      </c>
       <c r="D2" s="5" t="n"/>
       <c r="E2" s="5" t="n"/>
       <c r="F2" s="5" t="n"/>
@@ -31710,7 +31729,10 @@
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!I:I, "Yes")</f>
         <v/>
       </c>
-      <c r="C3" s="5" t="n"/>
+      <c r="C3" s="5">
+        <f>SPARKLINE('Monthly Summary'!C2:C100, {"charttype","line"; "color","red"})</f>
+        <v/>
+      </c>
       <c r="D3" s="5" t="n"/>
       <c r="E3" s="5" t="n"/>
       <c r="F3" s="5" t="n"/>
@@ -31745,7 +31767,10 @@
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!J:J, "Yes")</f>
         <v/>
       </c>
-      <c r="C4" s="5" t="n"/>
+      <c r="C4" s="5">
+        <f>SPARKLINE('Monthly Summary'!D2:D100, {"charttype","line"; "color","orange"})</f>
+        <v/>
+      </c>
       <c r="D4" s="5" t="n"/>
       <c r="E4" s="5" t="n"/>
       <c r="F4" s="5" t="n"/>
@@ -31869,9 +31894,19 @@
       <c r="Z7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n"/>
-      <c r="B8" s="5" t="n"/>
-      <c r="C8" s="5" t="n"/>
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Remaining Balance (After Bills)</t>
+        </is>
+      </c>
+      <c r="B8" s="5">
+        <f>INDEX('Monthly Summary'!F:F, MATCH(TEXT(TODAY(),"MMM-YYYY"),'Monthly Summary'!A:A,0))</f>
+        <v/>
+      </c>
+      <c r="C8" s="5">
+        <f>SPARKLINE('Monthly Summary'!F2:F100, {"charttype","line"; "color","green"})</f>
+        <v/>
+      </c>
       <c r="D8" s="5" t="n"/>
       <c r="E8" s="5" t="n"/>
       <c r="F8" s="5" t="n"/>
@@ -44076,6 +44111,14 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="cellIs" priority="1" operator="lessThan" dxfId="4" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" dxfId="5" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -44097,93 +44140,101 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>Net</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="0" t="inlineStr">
         <is>
           <t>Carryover</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="0" t="inlineStr">
         <is>
-          <t>Balance</t>
+          <t>Remaining Balance</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>Jan-2025</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <f>SUMIFS(Income!C:C, Income!D:D, A2)</f>
         <v/>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A2)</f>
         <v/>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <f>B2-C2</f>
         <v/>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="0" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <f>D2+E2</f>
         <v/>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>Feb-2025</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <f>SUMIFS(Income!C:C, Income!D:D, A3)</f>
         <v/>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A3)</f>
         <v/>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <f>B3-C3</f>
         <v/>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <f>F2</f>
         <v/>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <f>D3+E3</f>
         <v/>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F100">
+    <cfRule type="cellIs" priority="1" operator="lessThan" dxfId="4" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" dxfId="5" stopIfTrue="1">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Budget_Tracker_2025.xlsx with rebuilt Monthly Summary and error-free Dashboard
</commit_message>
<xml_diff>
--- a/assets/Budget_Tracker_2025.xlsx
+++ b/assets/Budget_Tracker_2025.xlsx
@@ -503,7 +503,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="4">
     <dxf>
       <font/>
       <fill>
@@ -540,22 +540,6 @@
         </patternFill>
       </fill>
       <border/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFC7CE"/>
-          <bgColor rgb="00FFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00C6EFCE"/>
-          <bgColor rgb="00C6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
@@ -763,7 +747,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
           </a:p>
         </txPr>
@@ -837,7 +821,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
           </a:p>
         </txPr>
@@ -860,7 +844,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t>None</a:t>
+            <a:t/>
           </a:r>
         </a:p>
       </txPr>
@@ -1383,7 +1367,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t>None</a:t>
+            <a:t/>
           </a:r>
         </a:p>
       </txPr>
@@ -1521,7 +1505,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
           </a:p>
         </txPr>
@@ -1595,7 +1579,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
           </a:p>
         </txPr>
@@ -1618,7 +1602,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t>None</a:t>
+            <a:t/>
           </a:r>
         </a:p>
       </txPr>
@@ -1957,37 +1941,37 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="35" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Item</t>
         </is>
       </c>
-      <c r="C1" s="35" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="D1" s="35" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="E1" s="35" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Days Until Due</t>
         </is>
       </c>
-      <c r="F1" s="35" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="G1" s="35" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Paid?</t>
         </is>
       </c>
-      <c r="H1" s="35" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
@@ -2032,28 +2016,28 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C2" s="38" t="n">
+      <c r="C2" s="9" t="n">
         <v>96.19</v>
       </c>
-      <c r="D2" s="38" t="inlineStr">
+      <c r="D2" s="9" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E2" s="38" t="n">
+      <c r="E2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="38" t="inlineStr">
+      <c r="F2" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="G2" s="38" t="inlineStr">
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H2" s="38" t="n"/>
+      <c r="H2" s="9" t="n"/>
       <c r="I2" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2093,28 +2077,28 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C3" s="38" t="n">
+      <c r="C3" s="9" t="n">
         <v>181.75</v>
       </c>
-      <c r="D3" s="41" t="inlineStr">
+      <c r="D3" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E3" s="38" t="n">
+      <c r="E3" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="41" t="inlineStr">
+      <c r="F3" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="G3" s="41" t="inlineStr">
+      <c r="G3" s="15" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H3" s="38" t="n"/>
+      <c r="H3" s="9" t="n"/>
       <c r="I3" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2148,12 +2132,12 @@
     <row r="4" hidden="1" s="57">
       <c r="A4" s="26" t="n"/>
       <c r="B4" s="18" t="n"/>
-      <c r="C4" s="38" t="n"/>
-      <c r="D4" s="38" t="n"/>
-      <c r="E4" s="38" t="n"/>
-      <c r="F4" s="38" t="n"/>
-      <c r="G4" s="38" t="n"/>
-      <c r="H4" s="38" t="n"/>
+      <c r="C4" s="9" t="n"/>
+      <c r="D4" s="9" t="n"/>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+      <c r="G4" s="9" t="n"/>
+      <c r="H4" s="9" t="n"/>
       <c r="I4" s="19">
         <f>IF(AND(A4&gt;=TODAY(), A4&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2191,28 +2175,28 @@
           <t>Car Payment</t>
         </is>
       </c>
-      <c r="C5" s="38" t="n">
+      <c r="C5" s="9" t="n">
         <v>547.9</v>
       </c>
-      <c r="D5" s="38" t="inlineStr">
+      <c r="D5" s="9" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E5" s="38" t="n">
+      <c r="E5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="38" t="inlineStr">
+      <c r="F5" s="9" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G5" s="38" t="inlineStr">
+      <c r="G5" s="9" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H5" s="38" t="n"/>
+      <c r="H5" s="9" t="n"/>
       <c r="I5" s="19">
         <f>IF(AND(A5&gt;=TODAY(), A5&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2250,28 +2234,28 @@
           <t>Rent Plan (Back)</t>
         </is>
       </c>
-      <c r="C6" s="38" t="n">
+      <c r="C6" s="9" t="n">
         <v>142</v>
       </c>
-      <c r="D6" s="41" t="inlineStr">
+      <c r="D6" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E6" s="38" t="n">
+      <c r="E6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="41" t="inlineStr">
+      <c r="F6" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="G6" s="41" t="inlineStr">
+      <c r="G6" s="15" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H6" s="38" t="n"/>
+      <c r="H6" s="9" t="n"/>
       <c r="I6" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -2311,24 +2295,24 @@
           <t>affirm</t>
         </is>
       </c>
-      <c r="C7" s="38" t="n">
+      <c r="C7" s="9" t="n">
         <v>36.46</v>
       </c>
-      <c r="D7" s="41" t="inlineStr">
+      <c r="D7" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E7" s="38" t="n">
+      <c r="E7" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="41" t="n"/>
-      <c r="G7" s="41" t="inlineStr">
+      <c r="F7" s="15" t="n"/>
+      <c r="G7" s="15" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H7" s="38" t="n"/>
+      <c r="H7" s="9" t="n"/>
       <c r="I7" s="23">
         <f>IF(AND(A7&gt;=TODAY(), A7&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2366,24 +2350,24 @@
           <t>affirm</t>
         </is>
       </c>
-      <c r="C8" s="38" t="n">
+      <c r="C8" s="9" t="n">
         <v>86.09</v>
       </c>
-      <c r="D8" s="41" t="inlineStr">
+      <c r="D8" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E8" s="38" t="n">
+      <c r="E8" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="38" t="n"/>
-      <c r="G8" s="38" t="inlineStr">
+      <c r="F8" s="9" t="n"/>
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H8" s="38" t="n"/>
+      <c r="H8" s="9" t="n"/>
       <c r="I8" s="19">
         <f>IF(AND(A8&gt;=TODAY(), A8&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2421,24 +2405,24 @@
           <t xml:space="preserve">Rent  </t>
         </is>
       </c>
-      <c r="C9" s="38" t="n">
+      <c r="C9" s="9" t="n">
         <v>2004</v>
       </c>
-      <c r="D9" s="41" t="inlineStr">
+      <c r="D9" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E9" s="38" t="n">
+      <c r="E9" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="41" t="n"/>
-      <c r="G9" s="41" t="inlineStr">
+      <c r="F9" s="15" t="n"/>
+      <c r="G9" s="15" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H9" s="38" t="n"/>
+      <c r="H9" s="9" t="n"/>
       <c r="I9" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2471,16 +2455,16 @@
     <row r="10" hidden="1" s="57">
       <c r="A10" s="26" t="n"/>
       <c r="B10" s="18" t="n"/>
-      <c r="C10" s="38" t="n"/>
-      <c r="D10" s="41" t="inlineStr">
+      <c r="C10" s="9" t="n"/>
+      <c r="D10" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E10" s="38" t="n"/>
-      <c r="F10" s="38" t="n"/>
-      <c r="G10" s="38" t="n"/>
-      <c r="H10" s="38" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+      <c r="G10" s="9" t="n"/>
+      <c r="H10" s="9" t="n"/>
       <c r="I10" s="19">
         <f>IF(AND(A10&gt;=TODAY(), A10&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2518,28 +2502,28 @@
           <t>Flight Ticket</t>
         </is>
       </c>
-      <c r="C11" s="38" t="n">
+      <c r="C11" s="9" t="n">
         <v>1200</v>
       </c>
-      <c r="D11" s="41" t="inlineStr">
+      <c r="D11" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E11" s="38" t="n">
+      <c r="E11" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="F11" s="38" t="inlineStr">
+      <c r="F11" s="9" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G11" s="38" t="inlineStr">
+      <c r="G11" s="9" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="H11" s="38" t="n"/>
+      <c r="H11" s="9" t="n"/>
       <c r="I11" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2578,28 +2562,28 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C12" s="38" t="n">
+      <c r="C12" s="9" t="n">
         <v>86.09</v>
       </c>
-      <c r="D12" s="41" t="inlineStr">
+      <c r="D12" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E12" s="38" t="n">
+      <c r="E12" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="F12" s="41" t="inlineStr">
+      <c r="F12" s="15" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G12" s="41" t="inlineStr">
+      <c r="G12" s="15" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="H12" s="38" t="n"/>
+      <c r="H12" s="9" t="n"/>
       <c r="I12" s="23">
         <f>IF(AND(A12&gt;=TODAY(), A12&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2637,28 +2621,28 @@
           <t>October Rent</t>
         </is>
       </c>
-      <c r="C13" s="38" t="n">
+      <c r="C13" s="9" t="n">
         <v>2052.09</v>
       </c>
-      <c r="D13" s="41" t="inlineStr">
+      <c r="D13" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E13" s="38" t="n">
+      <c r="E13" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="F13" s="38" t="inlineStr">
+      <c r="F13" s="9" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G13" s="38" t="inlineStr">
+      <c r="G13" s="9" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H13" s="38" t="n"/>
+      <c r="H13" s="9" t="n"/>
       <c r="I13" s="19">
         <f>IF(AND(A13&gt;=TODAY(), A13&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2696,28 +2680,28 @@
           <t>Capital One</t>
         </is>
       </c>
-      <c r="C14" s="38" t="n">
+      <c r="C14" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="D14" s="41" t="inlineStr">
+      <c r="D14" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E14" s="38" t="n">
+      <c r="E14" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="F14" s="41" t="inlineStr">
+      <c r="F14" s="15" t="inlineStr">
         <is>
           <t>Upcoming</t>
         </is>
       </c>
-      <c r="G14" s="41" t="inlineStr">
+      <c r="G14" s="15" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="H14" s="38" t="n"/>
+      <c r="H14" s="9" t="n"/>
       <c r="I14" s="23">
         <f>IF(AND(A14&gt;=TODAY(), A14&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2755,15 +2739,15 @@
           <t>FPL</t>
         </is>
       </c>
-      <c r="C15" s="38" t="n">
+      <c r="C15" s="9" t="n">
         <v>50.12</v>
       </c>
-      <c r="D15" s="41" t="inlineStr">
+      <c r="D15" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E15" s="38" t="n">
+      <c r="E15" s="9" t="n">
         <v>16</v>
       </c>
       <c r="F15" s="19" t="inlineStr">
@@ -2776,7 +2760,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H15" s="38" t="n"/>
+      <c r="H15" s="9" t="n"/>
       <c r="I15" s="19">
         <f>IF(AND(A15&gt;=TODAY(), A15&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2814,15 +2798,15 @@
           <t>Mazda</t>
         </is>
       </c>
-      <c r="C16" s="38" t="n">
+      <c r="C16" s="9" t="n">
         <v>308</v>
       </c>
-      <c r="D16" s="41" t="inlineStr">
+      <c r="D16" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E16" s="38" t="n">
+      <c r="E16" s="9" t="n">
         <v>28</v>
       </c>
       <c r="F16" s="23" t="inlineStr">
@@ -2835,7 +2819,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H16" s="38" t="n"/>
+      <c r="H16" s="9" t="n"/>
       <c r="I16" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -2874,15 +2858,15 @@
           <t>Mariner</t>
         </is>
       </c>
-      <c r="C17" s="38" t="n">
+      <c r="C17" s="9" t="n">
         <v>359</v>
       </c>
-      <c r="D17" s="38" t="inlineStr">
+      <c r="D17" s="9" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E17" s="38" t="n">
+      <c r="E17" s="9" t="n">
         <v>28</v>
       </c>
       <c r="F17" s="19" t="inlineStr">
@@ -2895,7 +2879,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H17" s="38" t="n"/>
+      <c r="H17" s="9" t="n"/>
       <c r="I17" s="19">
         <f>IF(AND(A17&gt;=TODAY(), A17&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2933,15 +2917,15 @@
           <t>JVT</t>
         </is>
       </c>
-      <c r="C18" s="38" t="n">
+      <c r="C18" s="9" t="n">
         <v>312</v>
       </c>
-      <c r="D18" s="41" t="inlineStr">
+      <c r="D18" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E18" s="38" t="n">
+      <c r="E18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="23" t="inlineStr">
@@ -2954,7 +2938,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H18" s="38" t="n"/>
+      <c r="H18" s="9" t="n"/>
       <c r="I18" s="23">
         <f>IF(AND(A18&gt;=TODAY(), A18&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -2992,15 +2976,15 @@
           <t>Miscellaneous</t>
         </is>
       </c>
-      <c r="C19" s="38" t="n">
+      <c r="C19" s="9" t="n">
         <v>89</v>
       </c>
-      <c r="D19" s="38" t="inlineStr">
+      <c r="D19" s="9" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E19" s="38" t="n">
+      <c r="E19" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="19" t="inlineStr">
@@ -3013,7 +2997,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H19" s="38" t="n"/>
+      <c r="H19" s="9" t="n"/>
       <c r="I19" s="19">
         <f>IF(AND(A19&gt;=TODAY(), A19&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3051,15 +3035,15 @@
           <t>Progressive</t>
         </is>
       </c>
-      <c r="C20" s="38" t="n">
+      <c r="C20" s="9" t="n">
         <v>179.66</v>
       </c>
-      <c r="D20" s="41" t="inlineStr">
+      <c r="D20" s="15" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E20" s="38" t="n">
+      <c r="E20" s="9" t="n">
         <v>4</v>
       </c>
       <c r="F20" s="23" t="inlineStr">
@@ -3072,7 +3056,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H20" s="38" t="n"/>
+      <c r="H20" s="9" t="n"/>
       <c r="I20" s="23">
         <f>IF(AND(A20&gt;=TODAY(), A20&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3110,15 +3094,15 @@
           <t>Alliance</t>
         </is>
       </c>
-      <c r="C21" s="38" t="n">
+      <c r="C21" s="9" t="n">
         <v>151</v>
       </c>
-      <c r="D21" s="38" t="inlineStr">
+      <c r="D21" s="9" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="E21" s="38" t="n">
+      <c r="E21" s="9" t="n">
         <v>4</v>
       </c>
       <c r="F21" s="19" t="inlineStr">
@@ -3131,7 +3115,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H21" s="38" t="n"/>
+      <c r="H21" s="9" t="n"/>
       <c r="I21" s="19">
         <f>IF(AND(A21&gt;=TODAY(), A21&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3169,15 +3153,15 @@
           <t>Sloan</t>
         </is>
       </c>
-      <c r="C22" s="38" t="n">
+      <c r="C22" s="9" t="n">
         <v>150.75</v>
       </c>
-      <c r="D22" s="41" t="inlineStr">
+      <c r="D22" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E22" s="38" t="n">
+      <c r="E22" s="9" t="n">
         <v>35</v>
       </c>
       <c r="F22" s="23" t="inlineStr">
@@ -3190,7 +3174,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H22" s="38" t="n"/>
+      <c r="H22" s="9" t="n"/>
       <c r="I22" s="23">
         <f>IF(AND(A22&gt;=TODAY(), A22&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3228,15 +3212,15 @@
           <t>Fortina</t>
         </is>
       </c>
-      <c r="C23" s="38" t="n">
+      <c r="C23" s="9" t="n">
         <v>40</v>
       </c>
-      <c r="D23" s="38" t="inlineStr">
+      <c r="D23" s="9" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E23" s="38" t="n">
+      <c r="E23" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F23" s="19" t="inlineStr">
@@ -3249,7 +3233,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H23" s="38" t="n"/>
+      <c r="H23" s="9" t="n"/>
       <c r="I23" s="19">
         <f>IF(AND(A23&gt;=TODAY(), A23&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3287,15 +3271,15 @@
           <t>Mariner</t>
         </is>
       </c>
-      <c r="C24" s="38" t="n">
+      <c r="C24" s="9" t="n">
         <v>359</v>
       </c>
-      <c r="D24" s="41" t="inlineStr">
+      <c r="D24" s="15" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E24" s="38" t="n">
+      <c r="E24" s="9" t="n">
         <v>30</v>
       </c>
       <c r="F24" s="23" t="inlineStr">
@@ -3308,7 +3292,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H24" s="38" t="n"/>
+      <c r="H24" s="9" t="n"/>
       <c r="I24" s="23">
         <f>IF(AND(A24&gt;=TODAY(), A24&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3346,15 +3330,15 @@
           <t>Adjustment</t>
         </is>
       </c>
-      <c r="C25" s="38" t="n">
+      <c r="C25" s="9" t="n">
         <v>652</v>
       </c>
-      <c r="D25" s="38" t="inlineStr">
+      <c r="D25" s="9" t="inlineStr">
         <is>
           <t>low</t>
         </is>
       </c>
-      <c r="E25" s="38" t="n">
+      <c r="E25" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="19" t="n"/>
@@ -3363,7 +3347,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H25" s="38" t="n"/>
+      <c r="H25" s="9" t="n"/>
       <c r="I25" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -3402,15 +3386,15 @@
           <t>Progressive</t>
         </is>
       </c>
-      <c r="C26" s="38" t="n">
+      <c r="C26" s="9" t="n">
         <v>179</v>
       </c>
-      <c r="D26" s="41" t="inlineStr">
+      <c r="D26" s="15" t="inlineStr">
         <is>
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E26" s="38" t="n">
+      <c r="E26" s="9" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="23" t="n"/>
@@ -3419,7 +3403,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H26" s="38" t="n"/>
+      <c r="H26" s="9" t="n"/>
       <c r="I26" s="23">
         <f>IF(AND(A26&gt;=TODAY(), A26&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3457,16 +3441,16 @@
           <t>Alliance</t>
         </is>
       </c>
-      <c r="C27" s="38">
+      <c r="C27" s="9">
         <f>155+25</f>
         <v/>
       </c>
-      <c r="D27" s="38" t="inlineStr">
+      <c r="D27" s="9" t="inlineStr">
         <is>
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E27" s="38" t="n">
+      <c r="E27" s="9" t="n">
         <v>1</v>
       </c>
       <c r="F27" s="19" t="n"/>
@@ -3475,7 +3459,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H27" s="38" t="n"/>
+      <c r="H27" s="9" t="n"/>
       <c r="I27" s="19">
         <f>IF(AND(A27&gt;=TODAY(), A27&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -3513,15 +3497,15 @@
           <t>car</t>
         </is>
       </c>
-      <c r="C28" s="38" t="n">
+      <c r="C28" s="9" t="n">
         <v>547.9</v>
       </c>
-      <c r="D28" s="41" t="inlineStr">
+      <c r="D28" s="15" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E28" s="38" t="n">
+      <c r="E28" s="9" t="n">
         <v>12</v>
       </c>
       <c r="F28" s="23" t="inlineStr">
@@ -3534,7 +3518,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H28" s="38" t="n"/>
+      <c r="H28" s="9" t="n"/>
       <c r="I28" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -3573,15 +3557,15 @@
           <t>Rent</t>
         </is>
       </c>
-      <c r="C29" s="38" t="n">
+      <c r="C29" s="9" t="n">
         <v>603</v>
       </c>
-      <c r="D29" s="38" t="inlineStr">
+      <c r="D29" s="9" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E29" s="38" t="n">
+      <c r="E29" s="9" t="n">
         <v>16</v>
       </c>
       <c r="F29" s="19" t="inlineStr">
@@ -3594,7 +3578,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H29" s="38" t="n"/>
+      <c r="H29" s="9" t="n"/>
       <c r="I29" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -3633,15 +3617,15 @@
           <t>Newera</t>
         </is>
       </c>
-      <c r="C30" s="38" t="n">
+      <c r="C30" s="9" t="n">
         <v>303</v>
       </c>
-      <c r="D30" s="41" t="inlineStr">
+      <c r="D30" s="15" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E30" s="38" t="n">
+      <c r="E30" s="9" t="n">
         <v>5</v>
       </c>
       <c r="F30" s="23" t="inlineStr">
@@ -3654,7 +3638,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H30" s="38" t="n"/>
+      <c r="H30" s="9" t="n"/>
       <c r="I30" s="23" t="inlineStr">
         <is>
           <t>yes</t>
@@ -3693,15 +3677,15 @@
           <t>Capital One</t>
         </is>
       </c>
-      <c r="C31" s="38" t="n">
+      <c r="C31" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="D31" s="41" t="inlineStr">
+      <c r="D31" s="15" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="E31" s="38" t="n">
+      <c r="E31" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="19" t="inlineStr">
@@ -3714,7 +3698,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H31" s="38" t="n"/>
+      <c r="H31" s="9" t="n"/>
       <c r="I31" s="19" t="inlineStr">
         <is>
           <t>yes</t>
@@ -3753,7 +3737,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C32" s="38" t="n">
+      <c r="C32" s="9" t="n">
         <v>181.75</v>
       </c>
       <c r="D32" s="23" t="inlineStr">
@@ -3761,7 +3745,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E32" s="38" t="n">
+      <c r="E32" s="9" t="n">
         <v>14</v>
       </c>
       <c r="F32" s="19" t="inlineStr">
@@ -3774,7 +3758,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H32" s="38" t="n"/>
+      <c r="H32" s="9" t="n"/>
       <c r="I32" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve"> no</t>
@@ -3813,7 +3797,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C33" s="38" t="n">
+      <c r="C33" s="9" t="n">
         <v>36.46</v>
       </c>
       <c r="D33" s="19" t="inlineStr">
@@ -3821,7 +3805,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E33" s="38" t="n">
+      <c r="E33" s="9" t="n">
         <v>14</v>
       </c>
       <c r="F33" s="19" t="inlineStr">
@@ -3834,7 +3818,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H33" s="38" t="n"/>
+      <c r="H33" s="9" t="n"/>
       <c r="I33" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -3873,7 +3857,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C34" s="38" t="n">
+      <c r="C34" s="9" t="n">
         <v>86.09</v>
       </c>
       <c r="D34" s="23" t="inlineStr">
@@ -3881,7 +3865,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E34" s="38" t="n">
+      <c r="E34" s="9" t="n">
         <v>14</v>
       </c>
       <c r="F34" s="19" t="inlineStr">
@@ -3894,7 +3878,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H34" s="38" t="n"/>
+      <c r="H34" s="9" t="n"/>
       <c r="I34" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -3933,7 +3917,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C35" s="38" t="n">
+      <c r="C35" s="9" t="n">
         <v>96.19</v>
       </c>
       <c r="D35" s="19" t="inlineStr">
@@ -3941,7 +3925,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E35" s="38" t="n">
+      <c r="E35" s="9" t="n">
         <v>14</v>
       </c>
       <c r="F35" s="19" t="inlineStr">
@@ -3954,7 +3938,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H35" s="38" t="n"/>
+      <c r="H35" s="9" t="n"/>
       <c r="I35" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -3993,7 +3977,7 @@
           <t>Affirm</t>
         </is>
       </c>
-      <c r="C36" s="38" t="n">
+      <c r="C36" s="9" t="n">
         <v>55.57</v>
       </c>
       <c r="D36" s="23" t="inlineStr">
@@ -4001,7 +3985,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E36" s="38" t="n">
+      <c r="E36" s="9" t="n">
         <v>14</v>
       </c>
       <c r="F36" s="19" t="inlineStr">
@@ -4014,7 +3998,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H36" s="38" t="n"/>
+      <c r="H36" s="9" t="n"/>
       <c r="I36" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -4053,7 +4037,7 @@
           <t>Rent</t>
         </is>
       </c>
-      <c r="C37" s="38" t="n">
+      <c r="C37" s="9" t="n">
         <v>142</v>
       </c>
       <c r="D37" s="19" t="inlineStr">
@@ -4061,7 +4045,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E37" s="38" t="n">
+      <c r="E37" s="9" t="n">
         <v>16</v>
       </c>
       <c r="F37" s="19" t="inlineStr">
@@ -4074,7 +4058,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H37" s="38" t="n"/>
+      <c r="H37" s="9" t="n"/>
       <c r="I37" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -4113,7 +4097,7 @@
           <t>Mariner</t>
         </is>
       </c>
-      <c r="C38" s="38" t="n">
+      <c r="C38" s="9" t="n">
         <v>359</v>
       </c>
       <c r="D38" s="23" t="inlineStr">
@@ -4121,7 +4105,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E38" s="38" t="n">
+      <c r="E38" s="9" t="n">
         <v>16</v>
       </c>
       <c r="F38" s="23" t="n"/>
@@ -4130,7 +4114,7 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="H38" s="38" t="n"/>
+      <c r="H38" s="9" t="n"/>
       <c r="I38" s="23">
         <f>IF(AND(A38&gt;=TODAY(), A38&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -4168,7 +4152,7 @@
           <t>Power</t>
         </is>
       </c>
-      <c r="C39" s="38" t="n">
+      <c r="C39" s="9" t="n">
         <v>0</v>
       </c>
       <c r="D39" s="19" t="inlineStr">
@@ -4176,7 +4160,7 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="E39" s="38" t="n">
+      <c r="E39" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F39" s="19" t="inlineStr">
@@ -4189,7 +4173,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H39" s="38" t="n"/>
+      <c r="H39" s="9" t="n"/>
       <c r="I39" s="19" t="inlineStr">
         <is>
           <t>no</t>
@@ -4228,7 +4212,7 @@
           <t>Cable</t>
         </is>
       </c>
-      <c r="C40" s="38" t="n">
+      <c r="C40" s="9" t="n">
         <v>0</v>
       </c>
       <c r="D40" s="23" t="inlineStr">
@@ -4236,7 +4220,7 @@
           <t>Medium</t>
         </is>
       </c>
-      <c r="E40" s="38" t="n">
+      <c r="E40" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="23" t="inlineStr">
@@ -4249,7 +4233,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H40" s="38" t="n"/>
+      <c r="H40" s="9" t="n"/>
       <c r="I40" s="23" t="inlineStr">
         <is>
           <t>no</t>
@@ -4289,7 +4273,7 @@
           <t>Ticket</t>
         </is>
       </c>
-      <c r="C41" s="38" t="n">
+      <c r="C41" s="9" t="n">
         <v>1200</v>
       </c>
       <c r="D41" s="19" t="inlineStr">
@@ -4297,7 +4281,7 @@
           <t>HIgh</t>
         </is>
       </c>
-      <c r="E41" s="38" t="n">
+      <c r="E41" s="9" t="n">
         <v>14</v>
       </c>
       <c r="F41" s="19" t="inlineStr">
@@ -4310,7 +4294,7 @@
           <t>no</t>
         </is>
       </c>
-      <c r="H41" s="38" t="n"/>
+      <c r="H41" s="9" t="n"/>
       <c r="I41" s="19" t="inlineStr">
         <is>
           <t>np</t>
@@ -4344,12 +4328,12 @@
     <row r="42" ht="15.75" customHeight="1" s="57">
       <c r="A42" s="26" t="n"/>
       <c r="B42" s="27" t="n"/>
-      <c r="C42" s="38" t="n"/>
+      <c r="C42" s="9" t="n"/>
       <c r="D42" s="23" t="n"/>
-      <c r="E42" s="38" t="n"/>
+      <c r="E42" s="9" t="n"/>
       <c r="F42" s="23" t="n"/>
       <c r="G42" s="23" t="n"/>
-      <c r="H42" s="38" t="n"/>
+      <c r="H42" s="9" t="n"/>
       <c r="I42" s="23">
         <f>IF(AND(A42&gt;=TODAY(), A42&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
@@ -4380,14 +4364,14 @@
     </row>
     <row r="43" ht="15.75" customHeight="1" s="57">
       <c r="A43" s="26" t="n"/>
-      <c r="B43" s="38" t="n"/>
-      <c r="C43" s="38" t="n"/>
+      <c r="B43" s="9" t="n"/>
+      <c r="C43" s="9" t="n"/>
       <c r="D43" s="19" t="n"/>
-      <c r="E43" s="38" t="n"/>
+      <c r="E43" s="9" t="n"/>
       <c r="F43" s="19" t="n"/>
       <c r="G43" s="23" t="n"/>
-      <c r="H43" s="38" t="n"/>
-      <c r="I43" s="38">
+      <c r="H43" s="9" t="n"/>
+      <c r="I43" s="9">
         <f>IF(AND(A43&gt;=TODAY(), A43&lt;=TODAY()+7), "Yes", "")</f>
         <v/>
       </c>
@@ -4418,12 +4402,12 @@
     <row r="44" ht="15.75" customHeight="1" s="57">
       <c r="A44" s="26" t="n"/>
       <c r="B44" s="21" t="n"/>
-      <c r="C44" s="38" t="n"/>
-      <c r="D44" s="38" t="n"/>
-      <c r="E44" s="38" t="n"/>
-      <c r="F44" s="38" t="n"/>
+      <c r="C44" s="9" t="n"/>
+      <c r="D44" s="9" t="n"/>
+      <c r="E44" s="9" t="n"/>
+      <c r="F44" s="9" t="n"/>
       <c r="G44" s="23" t="n"/>
-      <c r="H44" s="38" t="n"/>
+      <c r="H44" s="9" t="n"/>
       <c r="I44" s="21" t="n"/>
       <c r="J44" s="20" t="n"/>
       <c r="K44" s="17">
@@ -31691,10 +31675,7 @@
         <f>SUM(Income!C2:C100)</f>
         <v/>
       </c>
-      <c r="C2" s="5">
-        <f>SPARKLINE('Monthly Summary'!B2:B100, {"charttype","line"; "color","blue"})</f>
-        <v/>
-      </c>
+      <c r="C2" s="5" t="n"/>
       <c r="D2" s="5" t="n"/>
       <c r="E2" s="5" t="n"/>
       <c r="F2" s="5" t="n"/>
@@ -31729,10 +31710,7 @@
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!I:I, "Yes")</f>
         <v/>
       </c>
-      <c r="C3" s="5">
-        <f>SPARKLINE('Monthly Summary'!C2:C100, {"charttype","line"; "color","red"})</f>
-        <v/>
-      </c>
+      <c r="C3" s="5" t="n"/>
       <c r="D3" s="5" t="n"/>
       <c r="E3" s="5" t="n"/>
       <c r="F3" s="5" t="n"/>
@@ -31767,10 +31745,7 @@
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!J:J, "Yes")</f>
         <v/>
       </c>
-      <c r="C4" s="5">
-        <f>SPARKLINE('Monthly Summary'!D2:D100, {"charttype","line"; "color","orange"})</f>
-        <v/>
-      </c>
+      <c r="C4" s="5" t="n"/>
       <c r="D4" s="5" t="n"/>
       <c r="E4" s="5" t="n"/>
       <c r="F4" s="5" t="n"/>
@@ -31900,13 +31875,10 @@
         </is>
       </c>
       <c r="B8" s="5">
-        <f>INDEX('Monthly Summary'!F:F, MATCH(TEXT(TODAY(),"MMM-YYYY"),'Monthly Summary'!A:A,0))</f>
+        <f>INDEX('Monthly Summary'!F2:F13, MATCH(TEXT(TODAY(),"MMM-YYYY"), 'Monthly Summary'!A2:A13, 0))</f>
         <v/>
       </c>
-      <c r="C8" s="5">
-        <f>SPARKLINE('Monthly Summary'!F2:F100, {"charttype","line"; "color","green"})</f>
-        <v/>
-      </c>
+      <c r="C8" s="5" t="n"/>
       <c r="D8" s="5" t="n"/>
       <c r="E8" s="5" t="n"/>
       <c r="F8" s="5" t="n"/>
@@ -44111,14 +44083,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" priority="1" operator="lessThan" dxfId="4" stopIfTrue="1">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" dxfId="5" stopIfTrue="1">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -44131,7 +44095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44140,101 +44104,363 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Net</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Carryover</t>
         </is>
       </c>
-      <c r="F1" s="0" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Remaining Balance</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Jan-2025</t>
         </is>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <f>SUMIFS(Income!C:C, Income!D:D, A2)</f>
         <v/>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A2)</f>
         <v/>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <f>B2-C2</f>
         <v/>
       </c>
-      <c r="E2" s="0" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <f>D2+E2</f>
         <v/>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Feb-2025</t>
         </is>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <f>SUMIFS(Income!C:C, Income!D:D, A3)</f>
         <v/>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A3)</f>
         <v/>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <f>B3-C3</f>
         <v/>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <f>F2</f>
         <v/>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <f>D3+E3</f>
         <v/>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mar-2025</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>SUMIFS(Income!C:C, Income!D:D, A4)</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A4)</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>B4-C4</f>
+        <v/>
+      </c>
+      <c r="E4">
+        <f>F3</f>
+        <v/>
+      </c>
+      <c r="F4">
+        <f>D4+E4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Apr-2025</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>SUMIFS(Income!C:C, Income!D:D, A5)</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A5)</f>
+        <v/>
+      </c>
+      <c r="D5">
+        <f>B5-C5</f>
+        <v/>
+      </c>
+      <c r="E5">
+        <f>F4</f>
+        <v/>
+      </c>
+      <c r="F5">
+        <f>D5+E5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>May-2025</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>SUMIFS(Income!C:C, Income!D:D, A6)</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A6)</f>
+        <v/>
+      </c>
+      <c r="D6">
+        <f>B6-C6</f>
+        <v/>
+      </c>
+      <c r="E6">
+        <f>F5</f>
+        <v/>
+      </c>
+      <c r="F6">
+        <f>D6+E6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Jun-2025</t>
+        </is>
+      </c>
+      <c r="B7">
+        <f>SUMIFS(Income!C:C, Income!D:D, A7)</f>
+        <v/>
+      </c>
+      <c r="C7">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A7)</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>B7-C7</f>
+        <v/>
+      </c>
+      <c r="E7">
+        <f>F6</f>
+        <v/>
+      </c>
+      <c r="F7">
+        <f>D7+E7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jul-2025</t>
+        </is>
+      </c>
+      <c r="B8">
+        <f>SUMIFS(Income!C:C, Income!D:D, A8)</f>
+        <v/>
+      </c>
+      <c r="C8">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A8)</f>
+        <v/>
+      </c>
+      <c r="D8">
+        <f>B8-C8</f>
+        <v/>
+      </c>
+      <c r="E8">
+        <f>F7</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>D8+E8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Aug-2025</t>
+        </is>
+      </c>
+      <c r="B9">
+        <f>SUMIFS(Income!C:C, Income!D:D, A9)</f>
+        <v/>
+      </c>
+      <c r="C9">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A9)</f>
+        <v/>
+      </c>
+      <c r="D9">
+        <f>B9-C9</f>
+        <v/>
+      </c>
+      <c r="E9">
+        <f>F8</f>
+        <v/>
+      </c>
+      <c r="F9">
+        <f>D9+E9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sep-2025</t>
+        </is>
+      </c>
+      <c r="B10">
+        <f>SUMIFS(Income!C:C, Income!D:D, A10)</f>
+        <v/>
+      </c>
+      <c r="C10">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A10)</f>
+        <v/>
+      </c>
+      <c r="D10">
+        <f>B10-C10</f>
+        <v/>
+      </c>
+      <c r="E10">
+        <f>F9</f>
+        <v/>
+      </c>
+      <c r="F10">
+        <f>D10+E10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Oct-2025</t>
+        </is>
+      </c>
+      <c r="B11">
+        <f>SUMIFS(Income!C:C, Income!D:D, A11)</f>
+        <v/>
+      </c>
+      <c r="C11">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A11)</f>
+        <v/>
+      </c>
+      <c r="D11">
+        <f>B11-C11</f>
+        <v/>
+      </c>
+      <c r="E11">
+        <f>F10</f>
+        <v/>
+      </c>
+      <c r="F11">
+        <f>D11+E11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Nov-2025</t>
+        </is>
+      </c>
+      <c r="B12">
+        <f>SUMIFS(Income!C:C, Income!D:D, A12)</f>
+        <v/>
+      </c>
+      <c r="C12">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A12)</f>
+        <v/>
+      </c>
+      <c r="D12">
+        <f>B12-C12</f>
+        <v/>
+      </c>
+      <c r="E12">
+        <f>F11</f>
+        <v/>
+      </c>
+      <c r="F12">
+        <f>D12+E12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dec-2025</t>
+        </is>
+      </c>
+      <c r="B13">
+        <f>SUMIFS(Income!C:C, Income!D:D, A13)</f>
+        <v/>
+      </c>
+      <c r="C13">
+        <f>SUMIFS('Budget Tracker'!C:C, 'Budget Tracker'!L:L, A13)</f>
+        <v/>
+      </c>
+      <c r="D13">
+        <f>B13-C13</f>
+        <v/>
+      </c>
+      <c r="E13">
+        <f>F12</f>
+        <v/>
+      </c>
+      <c r="F13">
+        <f>D13+E13</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F100">
-    <cfRule type="cellIs" priority="1" operator="lessThan" dxfId="4" stopIfTrue="1">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" dxfId="5" stopIfTrue="1">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>